<commit_message>
add ko 470 test
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALVATORE\Desktop\Accreditamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALVATORE\Desktop\lavoro\anatomia patologica\MGSOFTXX_CERT\it-fse-accreditamento\GATEWAY\A1#111#MGSOFTXX\MGSOFT\websapfse\1.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="484">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1850,6 +1850,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Received HTTP response headers after 1062.9568ms - 201</t>
+  </si>
+  <si>
+    <t>Errore generato omettendo  il claim richesto</t>
+  </si>
+  <si>
+    <t>Errore generato valorizzando in modo errato  il claim richesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifica connessione </t>
+  </si>
+  <si>
+    <t>Correzione elemento mancante</t>
   </si>
 </sst>
 </file>
@@ -2331,7 +2343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2459,6 +2471,9 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3933,26 +3948,28 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D148" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T149" sqref="T149"/>
+      <selection pane="bottomRight" activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
     <col min="5" max="5" width="104.85546875" customWidth="1"/>
     <col min="6" max="8" width="33.140625" customWidth="1"/>
     <col min="9" max="9" width="55.42578125" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="11" width="45" customWidth="1"/>
     <col min="12" max="12" width="49.42578125" customWidth="1"/>
-    <col min="13" max="18" width="36.42578125" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" customWidth="1"/>
+    <col min="13" max="14" width="36.42578125" customWidth="1"/>
+    <col min="15" max="15" width="65" customWidth="1"/>
+    <col min="16" max="18" width="36.42578125" customWidth="1"/>
+    <col min="19" max="19" width="39" customWidth="1"/>
     <col min="20" max="20" width="33.140625" customWidth="1"/>
     <col min="21" max="21" width="36.42578125" customWidth="1"/>
     <col min="22" max="23" width="31.85546875" customWidth="1"/>
@@ -3981,12 +3998,12 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="52"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4007,14 +4024,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="60" t="s">
         <v>437</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="52"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4035,12 +4052,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="59" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="60" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4062,12 +4079,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="59" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4088,8 +4105,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -9467,7 +9484,9 @@
       <c r="J150" s="38" t="s">
         <v>442</v>
       </c>
-      <c r="K150" s="38"/>
+      <c r="K150" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L150" s="38"/>
       <c r="M150" s="38"/>
       <c r="N150" s="38"/>
@@ -9525,10 +9544,18 @@
       <c r="O151" s="38" t="s">
         <v>443</v>
       </c>
-      <c r="P151" s="38"/>
-      <c r="Q151" s="38"/>
-      <c r="R151" s="38"/>
-      <c r="S151" s="38"/>
+      <c r="P151" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q151" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R151" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S151" s="38" t="s">
+        <v>480</v>
+      </c>
       <c r="T151" s="38"/>
       <c r="U151" s="39"/>
       <c r="V151" s="40"/>
@@ -9561,21 +9588,33 @@
       <c r="H152" s="37" t="s">
         <v>461</v>
       </c>
-      <c r="I152" s="42" t="s">
-        <v>445</v>
-      </c>
-      <c r="J152" s="38"/>
+      <c r="I152" s="42"/>
+      <c r="J152" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K152" s="38"/>
       <c r="L152" s="38"/>
-      <c r="M152" s="38"/>
-      <c r="N152" s="38"/>
+      <c r="M152" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N152" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O152" s="38" t="s">
         <v>447</v>
       </c>
-      <c r="P152" s="38"/>
-      <c r="Q152" s="38"/>
-      <c r="R152" s="38"/>
-      <c r="S152" s="38"/>
+      <c r="P152" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q152" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R152" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S152" s="38" t="s">
+        <v>481</v>
+      </c>
       <c r="T152" s="38"/>
       <c r="U152" s="39"/>
       <c r="V152" s="40"/>
@@ -9607,8 +9646,12 @@
       </c>
       <c r="H153" s="37"/>
       <c r="I153" s="42"/>
-      <c r="J153" s="38"/>
-      <c r="K153" s="38"/>
+      <c r="J153" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K153" s="38" t="s">
+        <v>234</v>
+      </c>
       <c r="L153" s="38"/>
       <c r="M153" s="38" t="s">
         <v>228</v>
@@ -9629,7 +9672,7 @@
         <v>441</v>
       </c>
       <c r="S153" s="38" t="s">
-        <v>441</v>
+        <v>482</v>
       </c>
       <c r="T153" s="38"/>
       <c r="U153" s="39"/>
@@ -9673,7 +9716,9 @@
       </c>
       <c r="K154" s="38"/>
       <c r="L154" s="38"/>
-      <c r="M154" s="38"/>
+      <c r="M154" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="N154" s="38" t="s">
         <v>228</v>
       </c>
@@ -9683,9 +9728,15 @@
       <c r="P154" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q154" s="38"/>
-      <c r="R154" s="38"/>
-      <c r="S154" s="38"/>
+      <c r="Q154" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R154" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S154" s="38" t="s">
+        <v>481</v>
+      </c>
       <c r="T154" s="38"/>
       <c r="U154" s="39"/>
       <c r="V154" s="40"/>
@@ -9713,8 +9764,12 @@
       <c r="G155" s="37"/>
       <c r="H155" s="37"/>
       <c r="I155" s="42"/>
-      <c r="J155" s="38"/>
-      <c r="K155" s="38"/>
+      <c r="J155" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="K155" s="38" t="s">
+        <v>238</v>
+      </c>
       <c r="L155" s="38"/>
       <c r="M155" s="38"/>
       <c r="N155" s="38"/>
@@ -9763,13 +9818,25 @@
       </c>
       <c r="K156" s="38"/>
       <c r="L156" s="38"/>
-      <c r="M156" s="38"/>
-      <c r="N156" s="38"/>
+      <c r="M156" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N156" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O156" s="38"/>
-      <c r="P156" s="38"/>
-      <c r="Q156" s="38"/>
-      <c r="R156" s="38"/>
-      <c r="S156" s="38"/>
+      <c r="P156" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q156" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R156" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S156" s="38" t="s">
+        <v>481</v>
+      </c>
       <c r="T156" s="38"/>
       <c r="U156" s="39"/>
       <c r="V156" s="40"/>
@@ -9800,7 +9867,9 @@
       <c r="J157" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K157" s="38"/>
+      <c r="K157" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L157" s="38"/>
       <c r="M157" s="38"/>
       <c r="N157" s="38"/>
@@ -9839,7 +9908,9 @@
       <c r="J158" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K158" s="38"/>
+      <c r="K158" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L158" s="38"/>
       <c r="M158" s="38"/>
       <c r="N158" s="38"/>
@@ -9878,7 +9949,9 @@
       <c r="J159" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K159" s="38"/>
+      <c r="K159" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L159" s="38"/>
       <c r="M159" s="38"/>
       <c r="N159" s="38"/>
@@ -9917,7 +9990,9 @@
       <c r="J160" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K160" s="38"/>
+      <c r="K160" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L160" s="38"/>
       <c r="M160" s="38"/>
       <c r="N160" s="38"/>
@@ -9953,8 +10028,12 @@
       <c r="G161" s="37"/>
       <c r="H161" s="37"/>
       <c r="I161" s="42"/>
-      <c r="J161" s="38"/>
-      <c r="K161" s="38"/>
+      <c r="J161" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="K161" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L161" s="38"/>
       <c r="M161" s="38"/>
       <c r="N161" s="38"/>
@@ -9990,8 +10069,12 @@
       <c r="G162" s="37"/>
       <c r="H162" s="37"/>
       <c r="I162" s="42"/>
-      <c r="J162" s="38"/>
-      <c r="K162" s="38"/>
+      <c r="J162" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="K162" s="38" t="s">
+        <v>233</v>
+      </c>
       <c r="L162" s="38"/>
       <c r="M162" s="38"/>
       <c r="N162" s="38"/>
@@ -10040,15 +10123,27 @@
       </c>
       <c r="K163" s="38"/>
       <c r="L163" s="38"/>
-      <c r="M163" s="38"/>
-      <c r="N163" s="38"/>
+      <c r="M163" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N163" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O163" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="P163" s="38"/>
-      <c r="Q163" s="38"/>
-      <c r="R163" s="38"/>
-      <c r="S163" s="38"/>
+      <c r="P163" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q163" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R163" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S163" s="38" t="s">
+        <v>483</v>
+      </c>
       <c r="T163" s="38"/>
       <c r="U163" s="39"/>
       <c r="V163" s="40"/>
@@ -10955,19 +11050,27 @@
       <c r="M187" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="N187" s="38"/>
+      <c r="N187" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="O187" s="38" t="s">
         <v>472</v>
       </c>
-      <c r="P187" s="38"/>
-      <c r="Q187" s="38"/>
-      <c r="R187" s="38"/>
-      <c r="S187" s="35"/>
+      <c r="P187" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q187" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R187" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S187" s="48" t="s">
+        <v>450</v>
+      </c>
       <c r="T187" s="38"/>
       <c r="U187" s="35"/>
-      <c r="V187" s="35" t="s">
-        <v>450</v>
-      </c>
+      <c r="V187" s="35"/>
       <c r="W187" s="35" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
nuova versione test ok
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALVATORE\Desktop\lavoro\anatomia patologica\MGSOFTXX_CERT\it-fse-accreditamento\GATEWAY\A1#111#MGSOFTXX\MGSOFT\websapfse\1.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fse\GATEWAY\A1#111#MGSOFTXX\MGSOFT\websapfse\1.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$192</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="484">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1825,34 +1825,43 @@
     <t>Correzione elemento mancante</t>
   </si>
   <si>
-    <t>2025-08-07T10:21:34.008067Z</t>
-  </si>
-  <si>
-    <t>2025-08-07T12:29:42.7403202Z</t>
-  </si>
-  <si>
-    <t>279af96a1071a5b3f66754d8f4dd5c87</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.180a2be636^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-08-08T09:47:36.9068061Z</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.507a82717e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>a5bb39ed0a95855070000b0bd8b3042f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.2076d93045^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>bf1098c0a916a5a7214aeec08a8a8cd0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.bf5c0885c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>5118520a253ce8009dddccada691099d</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:40:03.361703Z</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:43:07.7667758Z</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:45:24.5032173Z</t>
+  </si>
+  <si>
+    <t>2025-09-23T14:14:04.8808404Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.59beaf6b4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>42ab369abb6cf10d838293e6fb1522f8</t>
+  </si>
+  <si>
+    <t>08599be25893165af899261422131127</t>
+  </si>
+  <si>
+    <t>f4352f248f0ceefc4b4052c7eecad6d6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.e94575dbfb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.2255c1b0df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.d99c26bfe9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2824,7 +2833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3974,10 +3983,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="P163" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T177" sqref="T177"/>
+      <selection pane="bottomRight" activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9407,16 +9416,16 @@
         <v>293</v>
       </c>
       <c r="F148" s="48">
-        <v>45904</v>
+        <v>45923</v>
       </c>
       <c r="G148" s="51" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H148" s="51" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="I148" s="51" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="J148" s="49" t="s">
         <v>64</v>
@@ -9456,16 +9465,16 @@
         <v>292</v>
       </c>
       <c r="F149" s="37">
-        <v>45876</v>
+        <v>45923</v>
       </c>
       <c r="G149" s="45" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="H149" s="45" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="I149" s="45" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="J149" s="38" t="s">
         <v>441</v>
@@ -9504,16 +9513,22 @@
       <c r="E150" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="F150" s="37"/>
-      <c r="G150" s="37"/>
-      <c r="H150" s="37"/>
-      <c r="I150" s="42"/>
+      <c r="F150" s="37">
+        <v>45923</v>
+      </c>
+      <c r="G150" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="H150" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="I150" s="42" t="s">
+        <v>477</v>
+      </c>
       <c r="J150" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="K150" s="38" t="s">
-        <v>233</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="K150" s="38"/>
       <c r="L150" s="38"/>
       <c r="M150" s="38"/>
       <c r="N150" s="38"/>
@@ -9522,14 +9537,16 @@
       <c r="Q150" s="38"/>
       <c r="R150" s="38"/>
       <c r="S150" s="38"/>
-      <c r="T150" s="38"/>
+      <c r="T150" s="38" t="s">
+        <v>226</v>
+      </c>
       <c r="U150" s="39"/>
       <c r="V150" s="40"/>
       <c r="W150" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="92.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>423</v>
       </c>
@@ -9590,7 +9607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="128.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="128.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>424</v>
       </c>
@@ -9649,7 +9666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="124.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>425</v>
       </c>
@@ -9710,7 +9727,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -9771,7 +9788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -9812,7 +9829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -9871,7 +9888,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -9912,7 +9929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -9953,7 +9970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -9994,7 +10011,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -10035,7 +10052,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -10076,7 +10093,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -10117,7 +10134,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -10676,16 +10693,16 @@
         <v>366</v>
       </c>
       <c r="F177" s="37">
-        <v>45904</v>
-      </c>
-      <c r="G177" s="37" t="s">
+        <v>45923</v>
+      </c>
+      <c r="G177" s="45" t="s">
         <v>475</v>
       </c>
       <c r="H177" s="37" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="I177" s="42" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="J177" s="38" t="s">
         <v>441</v>
@@ -11041,7 +11058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="53.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>470</v>
       </c>
@@ -11067,7 +11084,7 @@
         <v>466</v>
       </c>
       <c r="I187" s="35" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J187" s="38" t="s">
         <v>64</v>
@@ -15308,6 +15325,11 @@
     <filterColumn colId="2">
       <filters>
         <filter val="RAP"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="22">
+      <filters>
+        <filter val="OK"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -15408,11 +15430,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G960"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15446,7 +15469,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -15460,7 +15483,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>37</v>
       </c>
@@ -15474,7 +15497,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
@@ -15488,7 +15511,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>39</v>
       </c>
@@ -15502,7 +15525,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
@@ -15516,7 +15539,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -15530,7 +15553,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -15544,7 +15567,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -15558,7 +15581,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>223</v>
       </c>
@@ -16540,7 +16563,13 @@
     <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:G10"/>
+  <autoFilter ref="A1:G11">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="RAP"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -17594,6 +17623,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17851,18 +17892,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -17873,6 +17902,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17891,23 +17937,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
richiesta accreditamento 24 10
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
@@ -1846,22 +1846,22 @@
     <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5ef54a5b94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-10-19T11:49:37.7064972Z</t>
-  </si>
-  <si>
-    <t>439154e96442c3a2887f055327bf0cab</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.9ca36ed7d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-19T11:48:03.9723019Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.894d352881^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8261d9d65a62d43bc7b3bc96f4eb90af</t>
+    <t>6ecea624e34fce0941499791d3479831</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52abeb75980db08e9eefbde326335ffc5e3ba8c7.894d352881^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-10-24T14:16:53.2992796Z</t>
+  </si>
+  <si>
+    <t>2025-10-24T14:09:27.6306704Z</t>
+  </si>
+  <si>
+    <t>4d77d523de08195480fbf459a11effce</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5a5b44ec97^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3986,10 +3986,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H177" sqref="H177"/>
+      <selection pane="bottomRight" activeCell="I177" sqref="I177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9517,16 +9517,16 @@
         <v>279</v>
       </c>
       <c r="F150" s="37">
-        <v>45949</v>
+        <v>45954</v>
       </c>
       <c r="G150" s="37" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H150" s="37" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="I150" s="42" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J150" s="38" t="s">
         <v>64</v>
@@ -10696,16 +10696,16 @@
         <v>366</v>
       </c>
       <c r="F177" s="37">
-        <v>45949</v>
+        <v>45954</v>
       </c>
       <c r="G177" s="52" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="H177" s="37" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="I177" s="42" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="J177" s="38" t="s">
         <v>441</v>
@@ -17626,6 +17626,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17883,42 +17904,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17941,9 +17930,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update library 06 _11
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
@@ -1846,22 +1846,22 @@
     <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5ef54a5b94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>6ecea624e34fce0941499791d3479831</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52abeb75980db08e9eefbde326335ffc5e3ba8c7.894d352881^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-24T14:16:53.2992796Z</t>
-  </si>
-  <si>
-    <t>2025-10-24T14:09:27.6306704Z</t>
-  </si>
-  <si>
-    <t>4d77d523de08195480fbf459a11effce</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5a5b44ec97^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.d98fb275ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>33ddcf36df43cafd267419fc7d18df2a</t>
+  </si>
+  <si>
+    <t>2025-11-05T11:29:10.4662531Z</t>
+  </si>
+  <si>
+    <t>2025-11-05T11:27:05.6748837Z</t>
+  </si>
+  <si>
+    <t>50f50cd63691d588918d53cdc89bb6d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.74378addb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2020,7 +2020,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -2364,12 +2364,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2510,9 +2523,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2534,6 +2544,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3986,7 +4005,7 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F148" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="I177" sqref="I177"/>
@@ -4037,12 +4056,12 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="56"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="55"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4063,14 +4082,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="64" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4091,12 +4110,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="64" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="63" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4118,12 +4137,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="64" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="55"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4144,8 +4163,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -9520,13 +9539,13 @@
         <v>45954</v>
       </c>
       <c r="G150" s="37" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H150" s="37" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="I150" s="42" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="J150" s="38" t="s">
         <v>64</v>
@@ -10660,7 +10679,7 @@
       </c>
       <c r="F176" s="37"/>
       <c r="G176" s="37"/>
-      <c r="H176" s="37"/>
+      <c r="H176" s="36"/>
       <c r="I176" s="42"/>
       <c r="J176" s="38"/>
       <c r="K176" s="38"/>
@@ -10696,16 +10715,16 @@
         <v>366</v>
       </c>
       <c r="F177" s="37">
-        <v>45954</v>
-      </c>
-      <c r="G177" s="52" t="s">
-        <v>481</v>
-      </c>
-      <c r="H177" s="37" t="s">
-        <v>482</v>
+        <v>45966</v>
+      </c>
+      <c r="G177" s="64" t="s">
+        <v>480</v>
+      </c>
+      <c r="H177" s="66" t="s">
+        <v>479</v>
       </c>
       <c r="I177" s="42" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="J177" s="38" t="s">
         <v>441</v>
@@ -10746,7 +10765,7 @@
       </c>
       <c r="F178" s="35"/>
       <c r="G178" s="35"/>
-      <c r="H178" s="35"/>
+      <c r="H178" s="65"/>
       <c r="I178" s="35"/>
       <c r="J178" s="38"/>
       <c r="K178" s="38"/>
@@ -17626,15 +17645,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -17644,6 +17654,15 @@
     <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17905,14 +17924,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17925,6 +17936,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Risposte dettagliate alla gestione errori
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MGSOFTXX/MGSOFT/websapfse/1.0.1/report-checklist.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="482">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1757,9 +1757,6 @@
  "status":400,"instance":"/validation/error",</t>
   </si>
   <si>
-    <t>Errore Gestito Offline prima dell'invio ad Fse, attraverso la validazione su Xsd</t>
-  </si>
-  <si>
     <t>Errore Gestito Offline prima dell'invio ad Fse</t>
   </si>
   <si>
@@ -1801,67 +1798,63 @@
         "status":422,</t>
   </si>
   <si>
-    <t xml:space="preserve">        "type":"/msg/semantic",
-        "title":"Errore semantico.",
+    <t>2025-06-27T13:44:57.73072Z</t>
+  </si>
+  <si>
+    <t>916559c7274805c2d0d6fb899f7cb863</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.507a82717e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:43:07.7667758Z</t>
+  </si>
+  <si>
+    <t>f4352f248f0ceefc4b4052c7eecad6d6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.2255c1b0df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
+  </si>
+  <si>
+    <t>2025-09-30T09:43:27.9796913Z</t>
+  </si>
+  <si>
+    <t>dfedf2eb1c4e8c42bf1c4c7241e7d2fc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5ef54a5b94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-11-05T11:27:05.6748837Z</t>
+  </si>
+  <si>
+    <t>50f50cd63691d588918d53cdc89bb6d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.74378addb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>dcb8f5896476c356a91e50442b18c68d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.f4fd95670a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-11-10T08:11:22.4982363Z</t>
+  </si>
+  <si>
+    <t>L’applicativo effettua una validazione preliminare del documento, inclusa la verifica XSD offline. Successivamente, in fase di invio, il servizio FSE segnala l’errore sul token JWT. L’errore viene notificato all’utente, che provvede a contattare il supporto tecnico. Dopo la rigenerazione o correzione del token, l’utente può effettuare un nuovo invio verso FSE.</t>
+  </si>
+  <si>
+    <t>L'utente provvede a contattare il supporto tecnico per una verifica del funzionamento del servizio cercando di individuare la causa della mancata conessione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "title":"Errore sintattico.",
         "detail":"[ERRORE-5| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'R' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'],[ERRORE-45| L'elemento 'id' deve contenere gli attributi @root ed @extension valorizzati.]",
         "status":422,"instance":"/validation/error",</t>
   </si>
   <si>
-    <t>2025-06-27T13:44:57.73072Z</t>
-  </si>
-  <si>
-    <t>916559c7274805c2d0d6fb899f7cb863</t>
-  </si>
-  <si>
-    <t>Errore generato omettendo  il claim richesto</t>
-  </si>
-  <si>
-    <t>Errore generato valorizzando in modo errato  il claim richesto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verifica connessione </t>
-  </si>
-  <si>
-    <t>Correzione elemento mancante</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.507a82717e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-09-23T13:43:07.7667758Z</t>
-  </si>
-  <si>
-    <t>f4352f248f0ceefc4b4052c7eecad6d6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.2255c1b0df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
-    <t>2025-09-30T09:43:27.9796913Z</t>
-  </si>
-  <si>
-    <t>dfedf2eb1c4e8c42bf1c4c7241e7d2fc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5ef54a5b94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-11-05T11:27:05.6748837Z</t>
-  </si>
-  <si>
-    <t>50f50cd63691d588918d53cdc89bb6d4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.74378addb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>dcb8f5896476c356a91e50442b18c68d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.f4fd95670a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-11-10T08:11:22.4982363Z</t>
+    <t>L’applicativo effettua una validazione preliminare del documento, inclusa la verifica XSD offline. Il servizio segnala l’errore e viene notificato all’utente, che provvede a contattare il supporto tecnico. Dopo la verifica e la risoluzione del probolema, l’utente può effettuare un nuovo invio verso FSE.</t>
   </si>
 </sst>
 </file>
@@ -4005,10 +3998,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="O151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G177" sqref="G177"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9421,7 +9414,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" ht="54.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="35">
         <v>417</v>
       </c>
@@ -9441,13 +9434,13 @@
         <v>45930</v>
       </c>
       <c r="G148" s="51" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="H148" s="51" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="I148" s="51" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="J148" s="49" t="s">
         <v>64</v>
@@ -9470,7 +9463,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="35">
         <v>418</v>
       </c>
@@ -9490,13 +9483,13 @@
         <v>45923</v>
       </c>
       <c r="G149" s="45" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="H149" s="45" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="I149" s="45" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="J149" s="38" t="s">
         <v>441</v>
@@ -9519,7 +9512,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" ht="49.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="35">
         <v>419</v>
       </c>
@@ -9539,13 +9532,13 @@
         <v>45954</v>
       </c>
       <c r="G150" s="37" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="H150" s="37" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="I150" s="42" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="J150" s="38" t="s">
         <v>64</v>
@@ -9568,7 +9561,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="92.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>423</v>
       </c>
@@ -9620,16 +9613,18 @@
         <v>64</v>
       </c>
       <c r="S151" s="38" t="s">
-        <v>467</v>
-      </c>
-      <c r="T151" s="38"/>
+        <v>481</v>
+      </c>
+      <c r="T151" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U151" s="39"/>
       <c r="V151" s="40"/>
       <c r="W151" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="128.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="128.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>424</v>
       </c>
@@ -9649,10 +9644,10 @@
         <v>45835</v>
       </c>
       <c r="G152" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="H152" s="37" t="s">
         <v>452</v>
-      </c>
-      <c r="H152" s="37" t="s">
-        <v>453</v>
       </c>
       <c r="I152" s="42"/>
       <c r="J152" s="38" t="s">
@@ -9679,16 +9674,18 @@
         <v>64</v>
       </c>
       <c r="S152" s="38" t="s">
-        <v>468</v>
-      </c>
-      <c r="T152" s="38"/>
+        <v>481</v>
+      </c>
+      <c r="T152" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U152" s="39"/>
       <c r="V152" s="40"/>
       <c r="W152" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="124.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>425</v>
       </c>
@@ -9738,18 +9735,20 @@
         <v>441</v>
       </c>
       <c r="S153" s="38" t="s">
-        <v>469</v>
-      </c>
-      <c r="T153" s="38"/>
+        <v>479</v>
+      </c>
+      <c r="T153" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U153" s="39"/>
       <c r="V153" s="40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="W153" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -9769,13 +9768,13 @@
         <v>45835</v>
       </c>
       <c r="G154" s="37" t="s">
+        <v>453</v>
+      </c>
+      <c r="H154" s="37" t="s">
         <v>454</v>
       </c>
-      <c r="H154" s="37" t="s">
+      <c r="I154" s="42" t="s">
         <v>455</v>
-      </c>
-      <c r="I154" s="42" t="s">
-        <v>456</v>
       </c>
       <c r="J154" s="38" t="s">
         <v>64</v>
@@ -9801,16 +9800,18 @@
         <v>64</v>
       </c>
       <c r="S154" s="38" t="s">
-        <v>468</v>
-      </c>
-      <c r="T154" s="38"/>
+        <v>481</v>
+      </c>
+      <c r="T154" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U154" s="39"/>
       <c r="V154" s="40"/>
       <c r="W154" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -9851,7 +9852,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -9871,13 +9872,13 @@
         <v>45835</v>
       </c>
       <c r="G156" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="H156" s="45" t="s">
         <v>457</v>
       </c>
-      <c r="H156" s="45" t="s">
+      <c r="I156" s="42" t="s">
         <v>458</v>
-      </c>
-      <c r="I156" s="42" t="s">
-        <v>459</v>
       </c>
       <c r="J156" s="38" t="s">
         <v>64</v>
@@ -9901,16 +9902,18 @@
         <v>64</v>
       </c>
       <c r="S156" s="38" t="s">
-        <v>468</v>
-      </c>
-      <c r="T156" s="38"/>
+        <v>478</v>
+      </c>
+      <c r="T156" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U156" s="39"/>
       <c r="V156" s="40"/>
       <c r="W156" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -9951,7 +9954,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -9992,7 +9995,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -10033,7 +10036,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -10074,7 +10077,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -10115,7 +10118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -10156,7 +10159,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -10176,13 +10179,13 @@
         <v>45835</v>
       </c>
       <c r="G163" s="45" t="s">
+        <v>459</v>
+      </c>
+      <c r="H163" s="45" t="s">
         <v>460</v>
       </c>
-      <c r="H163" s="45" t="s">
+      <c r="I163" s="42" t="s">
         <v>461</v>
-      </c>
-      <c r="I163" s="42" t="s">
-        <v>462</v>
       </c>
       <c r="J163" s="38" t="s">
         <v>64</v>
@@ -10196,7 +10199,7 @@
         <v>228</v>
       </c>
       <c r="O163" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P163" s="38" t="s">
         <v>64</v>
@@ -10208,9 +10211,11 @@
         <v>64</v>
       </c>
       <c r="S163" s="38" t="s">
-        <v>470</v>
-      </c>
-      <c r="T163" s="38"/>
+        <v>481</v>
+      </c>
+      <c r="T163" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U163" s="39"/>
       <c r="V163" s="40"/>
       <c r="W163" s="38" t="s">
@@ -10698,7 +10703,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="66" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="35">
         <v>460</v>
       </c>
@@ -10718,13 +10723,13 @@
         <v>45966</v>
       </c>
       <c r="G177" s="52" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="H177" s="54" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I177" s="42" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="J177" s="38" t="s">
         <v>441</v>
@@ -11080,7 +11085,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="53.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>470</v>
       </c>
@@ -11100,13 +11105,13 @@
         <v>45835</v>
       </c>
       <c r="G187" s="35" t="s">
+        <v>463</v>
+      </c>
+      <c r="H187" s="35" t="s">
+        <v>464</v>
+      </c>
+      <c r="I187" s="35" t="s">
         <v>465</v>
-      </c>
-      <c r="H187" s="35" t="s">
-        <v>466</v>
-      </c>
-      <c r="I187" s="35" t="s">
-        <v>471</v>
       </c>
       <c r="J187" s="38" t="s">
         <v>64</v>
@@ -11117,13 +11122,13 @@
         <v>64</v>
       </c>
       <c r="N187" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="O187" s="38" t="s">
+        <v>480</v>
+      </c>
+      <c r="P187" s="38" t="s">
         <v>64</v>
-      </c>
-      <c r="O187" s="38" t="s">
-        <v>464</v>
-      </c>
-      <c r="P187" s="38" t="s">
-        <v>228</v>
       </c>
       <c r="Q187" s="38" t="s">
         <v>228</v>
@@ -11132,9 +11137,11 @@
         <v>64</v>
       </c>
       <c r="S187" s="47" t="s">
-        <v>450</v>
-      </c>
-      <c r="T187" s="38"/>
+        <v>481</v>
+      </c>
+      <c r="T187" s="38" t="s">
+        <v>227</v>
+      </c>
       <c r="U187" s="35"/>
       <c r="V187" s="35"/>
       <c r="W187" s="35" t="s">
@@ -15351,7 +15358,7 @@
     </filterColumn>
     <filterColumn colId="22">
       <filters>
-        <filter val="OK"/>
+        <filter val="KO"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -17645,15 +17652,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -17663,6 +17661,15 @@
     <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17924,14 +17931,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17944,6 +17943,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>